<commit_message>
Changed name according to TICC-137
</commit_message>
<xml_diff>
--- a/publication/v7.1/Peppol Code Lists - Document types v7.1.xlsx
+++ b/publication/v7.1/Peppol Code Lists - Document types v7.1.xlsx
@@ -781,12 +781,6 @@
     <t>TICC-117; TICC-136</t>
   </si>
   <si>
-    <t>Agid Order</t>
-  </si>
-  <si>
-    <t>Agid Order Response</t>
-  </si>
-  <si>
     <t>TICC-137</t>
   </si>
   <si>
@@ -797,6 +791,12 @@
   </si>
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:OrderResponse-2::OrderResponse##urn:fdc:peppol.eu:poacc:trns:order_response:3:restrictive:urn:www.agid.gov.it:trns:risposta_ordine:3.0::2.1</t>
+  </si>
+  <si>
+    <t>SimpleOrder_IT</t>
+  </si>
+  <si>
+    <t>OrderResponse_IT</t>
   </si>
 </sst>
 </file>
@@ -1303,7 +1303,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A98" sqref="A98"/>
+      <selection pane="bottomLeft" activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -4389,13 +4389,13 @@
     </row>
     <row r="97" spans="1:11" ht="30">
       <c r="A97" s="3" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D97" s="9" t="s">
         <v>236</v>
@@ -4405,7 +4405,7 @@
         <v>0</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H97" s="3" t="b">
         <f>FALSE</f>
@@ -4415,18 +4415,18 @@
         <v>142</v>
       </c>
       <c r="K97" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="98" spans="1:11" ht="45">
       <c r="A98" s="3" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D98" s="9" t="s">
         <v>236</v>
@@ -4436,7 +4436,7 @@
         <v>0</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H98" s="3" t="b">
         <f>FALSE</f>

</xml_diff>